<commit_message>
Gut dass wir uns morgen treffen, denn dann muss ich das hier nicht bis 90 Uhr a.m. machen sondenr kann jan fragen haHA
</commit_message>
<xml_diff>
--- a/Ressourcen/mitarbeiterEquipment.xlsx
+++ b/Ressourcen/mitarbeiterEquipment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcoK\Documents\UiPath\apsolutProjektRepository\Ressourcen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C449E0B-C49D-4FC0-8C4C-2B04FFEB6F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2FC878-FD20-489E-ABFE-F3C1BFA0D316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,13 +54,13 @@
     <t>PC-01</t>
   </si>
   <si>
-    <t>RW-01</t>
-  </si>
-  <si>
     <t>MacBook, Arbeitskleidung für den Vertrieb</t>
   </si>
   <si>
-    <t xml:space="preserve">  PC-01 ,   AK-01</t>
+    <t xml:space="preserve">  PC-01 ,   AK-03</t>
+  </si>
+  <si>
+    <t>RW-02</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -416,10 +416,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -441,7 +441,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FEDDICH DEN SCHEISS ?!
</commit_message>
<xml_diff>
--- a/Ressourcen/mitarbeiterEquipment.xlsx
+++ b/Ressourcen/mitarbeiterEquipment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcoK\Documents\UiPath\apsolutProjektRepository\Ressourcen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Imran\Documents\UiPath\apsolutProjektRepository\Ressourcen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2FC878-FD20-489E-ABFE-F3C1BFA0D316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DEDEE6-68ED-4504-897A-4280307ABCB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
     <t xml:space="preserve">  PC-01 ,   AK-03</t>
   </si>
   <si>
-    <t>RW-02</t>
+    <t>RW-02, PC-01</t>
   </si>
 </sst>
 </file>
@@ -390,17 +390,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.36328125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -411,7 +411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -422,7 +422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -433,7 +433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>

</xml_diff>